<commit_message>
Atualização de processo de abertura de issue
</commit_message>
<xml_diff>
--- a/docs/UnitTesting_IssueMsg .xlsx
+++ b/docs/UnitTesting_IssueMsg .xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\venv\.__Projetos\Avalcorp\ESG_VM\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D8BC1CA-8A4B-45A8-89C9-8463777E1C06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A36AB082-B243-47E0-8EEA-9C4F99B7E1FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="11460" firstSheet="2" activeTab="3" xr2:uid="{AF37AB55-194C-4C17-A308-5DCA304A4FDA}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="98">
   <si>
     <t>ISSUE_ASSIGNEES_NAME</t>
   </si>
@@ -298,31 +298,55 @@
     <t>2. COMMENTS</t>
   </si>
   <si>
-    <t>3. PULL REQUEST</t>
-  </si>
-  <si>
-    <t>3.1. Testes automatizados: Dependendo do projeto, pode haver testes automatizados que são executados quando um pull request é criado.</t>
-  </si>
-  <si>
-    <t>4. PULL REQUEST ANSWER</t>
-  </si>
-  <si>
-    <t>5. PULL REQUEST ACCEPANCE</t>
-  </si>
-  <si>
-    <t>5.1. Merge de pull request: Depois que um pull request é aceito, ele precisa ser mesclado com o branch principal.</t>
-  </si>
-  <si>
-    <t>6. GISTS</t>
-  </si>
-  <si>
-    <t>7. CLOSE</t>
-  </si>
-  <si>
-    <t>7.1. Referenciando o pull request/commit que resolveu o issue: Quando um issue é resolvido, é uma boa prática referenciar o pull request ou commit que resolveu o issue.</t>
-  </si>
-  <si>
     <t>2.1. Atribuir a colaborador, a TASK relacionada ao COMMENTS</t>
+  </si>
+  <si>
+    <t>3. DoR</t>
+  </si>
+  <si>
+    <t>4. PULL REQUEST</t>
+  </si>
+  <si>
+    <t>4.1. Testes automatizados: Dependendo do projeto, pode haver testes automatizados que são executados quando um pull request é criado.</t>
+  </si>
+  <si>
+    <t>5. PULL REQUEST ANSWER</t>
+  </si>
+  <si>
+    <t>6. PULL REQUEST ACCEPANCE</t>
+  </si>
+  <si>
+    <t>6.1. Merge de pull request: Depois que um pull request é aceito, ele precisa ser mesclado com o branch principal.</t>
+  </si>
+  <si>
+    <t>7. GISTS</t>
+  </si>
+  <si>
+    <t>8. CLOSE</t>
+  </si>
+  <si>
+    <t>8.1. Referenciando o pull request/commit que resolveu o issue: Quando um issue é resolvido, é uma boa prática referenciar o pull request ou commit que resolveu o issue.</t>
+  </si>
+  <si>
+    <t>1.5. Criticality Defined</t>
+  </si>
+  <si>
+    <t>1.6. Skill Definition</t>
+  </si>
+  <si>
+    <t>1.7. Code of Conduct</t>
+  </si>
+  <si>
+    <t>Automatic</t>
+  </si>
+  <si>
+    <t>Manual</t>
+  </si>
+  <si>
+    <t>Manual (Sugestion ?)</t>
+  </si>
+  <si>
+    <t>Manual or rev_it</t>
   </si>
 </sst>
 </file>
@@ -455,12 +479,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -469,6 +487,12 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -994,30 +1018,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.75">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="18" t="s">
         <v>44</v>
       </c>
-      <c r="B1" s="15" t="s">
+      <c r="B1" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="C1" s="15" t="s">
+      <c r="C1" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="D1" s="15"/>
-      <c r="H1" s="15" t="s">
+      <c r="D1" s="18"/>
+      <c r="H1" s="18" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.75">
-      <c r="A2" s="15"/>
-      <c r="B2" s="15"/>
+      <c r="A2" s="18"/>
+      <c r="B2" s="18"/>
       <c r="C2" s="7" t="s">
         <v>36</v>
       </c>
       <c r="D2" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="H2" s="15"/>
+      <c r="H2" s="18"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A3" s="8" t="s">
@@ -1026,10 +1050,10 @@
       <c r="B3" s="9">
         <v>10</v>
       </c>
-      <c r="C3" s="16" t="s">
+      <c r="C3" s="19" t="s">
         <v>38</v>
       </c>
-      <c r="D3" s="16" t="s">
+      <c r="D3" s="19" t="s">
         <v>43</v>
       </c>
       <c r="H3" s="8" t="s">
@@ -1043,8 +1067,8 @@
       <c r="B4" s="9">
         <v>6</v>
       </c>
-      <c r="C4" s="16"/>
-      <c r="D4" s="16"/>
+      <c r="C4" s="19"/>
+      <c r="D4" s="19"/>
       <c r="H4" s="8" t="s">
         <v>46</v>
       </c>
@@ -1056,8 +1080,8 @@
       <c r="B5" s="9">
         <v>14</v>
       </c>
-      <c r="C5" s="16"/>
-      <c r="D5" s="16"/>
+      <c r="C5" s="19"/>
+      <c r="D5" s="19"/>
       <c r="H5" s="8" t="s">
         <v>47</v>
       </c>
@@ -1069,8 +1093,8 @@
       <c r="B6" s="9">
         <v>4</v>
       </c>
-      <c r="C6" s="16"/>
-      <c r="D6" s="16"/>
+      <c r="C6" s="19"/>
+      <c r="D6" s="19"/>
       <c r="H6" s="8" t="s">
         <v>48</v>
       </c>
@@ -1141,16 +1165,16 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{662486F5-DD9A-4C28-87E7-50C66D2DE293}">
-  <dimension ref="A1:I41"/>
+  <dimension ref="A1:I45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="A28" sqref="A28"/>
+    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
   <cols>
     <col min="1" max="1" width="56.04296875" customWidth="1"/>
-    <col min="2" max="2" width="12.54296875" customWidth="1"/>
+    <col min="2" max="2" width="17.86328125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.08984375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.1328125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.453125" bestFit="1" customWidth="1"/>
@@ -1161,22 +1185,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.75">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="18" t="s">
         <v>70</v>
       </c>
-      <c r="B1" s="15" t="s">
+      <c r="B1" s="18" t="s">
         <v>71</v>
       </c>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
-      <c r="G1" s="15"/>
-      <c r="H1" s="15"/>
-      <c r="I1" s="15"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
+      <c r="I1" s="18"/>
     </row>
     <row r="2" spans="1:9" ht="44.25" x14ac:dyDescent="0.75">
-      <c r="A2" s="15"/>
+      <c r="A2" s="18"/>
       <c r="B2" s="13" t="s">
         <v>57</v>
       </c>
@@ -1348,20 +1372,20 @@
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.75">
-      <c r="A9" s="15" t="s">
+      <c r="A9" s="18" t="s">
         <v>63</v>
       </c>
-      <c r="B9" s="15" t="s">
+      <c r="B9" s="18" t="s">
         <v>64</v>
       </c>
-      <c r="C9" s="15"/>
-      <c r="D9" s="15"/>
-      <c r="E9" s="15"/>
-      <c r="F9" s="15"/>
-      <c r="G9" s="15"/>
+      <c r="C9" s="18"/>
+      <c r="D9" s="18"/>
+      <c r="E9" s="18"/>
+      <c r="F9" s="18"/>
+      <c r="G9" s="18"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.75">
-      <c r="A10" s="15"/>
+      <c r="A10" s="18"/>
       <c r="B10" s="7" t="s">
         <v>65</v>
       </c>
@@ -1566,99 +1590,140 @@
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.75">
-      <c r="A21" s="15" t="s">
+      <c r="A21" s="18" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.75">
-      <c r="A22" s="15"/>
+      <c r="A22" s="18"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.75">
-      <c r="A23" s="17" t="s">
+      <c r="A23" s="15" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="44.25" x14ac:dyDescent="0.75">
-      <c r="A24" s="17" t="s">
+      <c r="A24" s="15" t="s">
         <v>76</v>
       </c>
+      <c r="B24" t="s">
+        <v>94</v>
+      </c>
     </row>
     <row r="25" spans="1:7" ht="29.5" x14ac:dyDescent="0.75">
-      <c r="A25" s="17" t="s">
+      <c r="A25" s="15" t="s">
         <v>77</v>
       </c>
+      <c r="B25" t="s">
+        <v>94</v>
+      </c>
     </row>
     <row r="26" spans="1:7" ht="44.25" x14ac:dyDescent="0.75">
-      <c r="A26" s="17" t="s">
+      <c r="A26" s="15" t="s">
         <v>78</v>
       </c>
+      <c r="B26" t="s">
+        <v>96</v>
+      </c>
     </row>
     <row r="27" spans="1:7" ht="44.25" x14ac:dyDescent="0.75">
-      <c r="A27" s="17" t="s">
+      <c r="A27" s="15" t="s">
         <v>79</v>
       </c>
+      <c r="B27" t="s">
+        <v>96</v>
+      </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.75">
-      <c r="A28" s="17" t="s">
+      <c r="A28" s="15" t="s">
+        <v>91</v>
+      </c>
+      <c r="B28" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.75">
+      <c r="A29" s="15" t="s">
+        <v>92</v>
+      </c>
+      <c r="B29" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.75">
+      <c r="A30" s="15" t="s">
+        <v>93</v>
+      </c>
+      <c r="B30" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.75">
+      <c r="A31" s="15" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.75">
-      <c r="A29" s="17" t="s">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.75">
+      <c r="A32" s="15" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.75">
+      <c r="A33" s="15" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.75">
+      <c r="A34" s="15" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" ht="44.25" x14ac:dyDescent="0.75">
+      <c r="A35" s="15" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.75">
+      <c r="A36" s="15" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.75">
+      <c r="A37" s="15" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" ht="29.5" x14ac:dyDescent="0.75">
+      <c r="A38" s="15" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.75">
+      <c r="A39" s="15" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.75">
+      <c r="A40" s="15" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.75">
-      <c r="A30" s="17" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" ht="44.25" x14ac:dyDescent="0.75">
-      <c r="A31" s="17" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.75">
-      <c r="A32" s="17" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.75">
-      <c r="A33" s="17" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="34" spans="1:1" ht="29.5" x14ac:dyDescent="0.75">
-      <c r="A34" s="17" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.75">
-      <c r="A35" s="17" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.75">
-      <c r="A36" s="17" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="37" spans="1:1" ht="44.25" x14ac:dyDescent="0.75">
-      <c r="A37" s="17" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="38" spans="1:1" ht="18.5" x14ac:dyDescent="0.75">
-      <c r="A38" s="19"/>
-    </row>
-    <row r="39" spans="1:1" ht="18.5" x14ac:dyDescent="0.75">
-      <c r="A39" s="19"/>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.75">
-      <c r="A40" s="17"/>
-    </row>
-    <row r="41" spans="1:1" ht="18.5" x14ac:dyDescent="0.75">
-      <c r="A41" s="18"/>
+    <row r="41" spans="1:1" ht="44.25" x14ac:dyDescent="0.75">
+      <c r="A41" s="15" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" ht="18.5" x14ac:dyDescent="0.75">
+      <c r="A42" s="17"/>
+    </row>
+    <row r="43" spans="1:1" ht="18.5" x14ac:dyDescent="0.75">
+      <c r="A43" s="17"/>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.75">
+      <c r="A44" s="15"/>
+    </row>
+    <row r="45" spans="1:1" ht="18.5" x14ac:dyDescent="0.75">
+      <c r="A45" s="16"/>
     </row>
   </sheetData>
   <mergeCells count="5">

</xml_diff>

<commit_message>
Atualizando Mapa de Fluxo
</commit_message>
<xml_diff>
--- a/docs/UnitTesting_IssueMsg .xlsx
+++ b/docs/UnitTesting_IssueMsg .xlsx
@@ -8,15 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\venv\.__Projetos\Avalcorp\ESG_VM\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A36AB082-B243-47E0-8EEA-9C4F99B7E1FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B0FFF70-EFDA-4711-ACC3-AAB1FCCFB4DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="11460" firstSheet="2" activeTab="3" xr2:uid="{AF37AB55-194C-4C17-A308-5DCA304A4FDA}"/>
+    <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="11460" tabRatio="811" firstSheet="1" activeTab="3" xr2:uid="{AF37AB55-194C-4C17-A308-5DCA304A4FDA}"/>
   </bookViews>
   <sheets>
     <sheet name="Testa Formato de Msg no Issue" sheetId="1" r:id="rId1"/>
     <sheet name="Tests em TreatIssue_Opening.yml" sheetId="2" r:id="rId2"/>
     <sheet name="Skills x Teams" sheetId="3" r:id="rId3"/>
     <sheet name="Issues Format and Responsabilit" sheetId="4" r:id="rId4"/>
+    <sheet name="Kanban Bug Issue" sheetId="5" r:id="rId5"/>
+    <sheet name="Kanban FReq Issue" sheetId="6" r:id="rId6"/>
+    <sheet name="Kanban NFReq Issue" sheetId="7" r:id="rId7"/>
+    <sheet name="Kanban Enabler Issue" sheetId="8" r:id="rId8"/>
+    <sheet name="Kanban Enhance Issue" sheetId="9" r:id="rId9"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="103">
   <si>
     <t>ISSUE_ASSIGNEES_NAME</t>
   </si>
@@ -292,12 +297,6 @@
     <t>1.3. Referenciando issues: Se um issue está relacionado a outro issue ou pull request, você pode referenciá-lo usando # seguido pelo número do issue.</t>
   </si>
   <si>
-    <t>1.4. Milestone do issue: Se o issue faz parte de um conjunto maior de tarefas ou projeto, você pode adicionar o issue a um milestone.</t>
-  </si>
-  <si>
-    <t>2. COMMENTS</t>
-  </si>
-  <si>
     <t>2.1. Atribuir a colaborador, a TASK relacionada ao COMMENTS</t>
   </si>
   <si>
@@ -319,9 +318,6 @@
     <t>6.1. Merge de pull request: Depois que um pull request é aceito, ele precisa ser mesclado com o branch principal.</t>
   </si>
   <si>
-    <t>7. GISTS</t>
-  </si>
-  <si>
     <t>8. CLOSE</t>
   </si>
   <si>
@@ -340,13 +336,57 @@
     <t>Automatic</t>
   </si>
   <si>
-    <t>Manual</t>
-  </si>
-  <si>
     <t>Manual (Sugestion ?)</t>
   </si>
   <si>
-    <t>Manual or rev_it</t>
+    <t>Manual (Check Automaticly)</t>
+  </si>
+  <si>
+    <t>Owner or rev_it</t>
+  </si>
+  <si>
+    <t>8.2. Release</t>
+  </si>
+  <si>
+    <t>2. COMMENTS (TASKs)</t>
+  </si>
+  <si>
+    <t>6.2. Tagging</t>
+  </si>
+  <si>
+    <t>7. GISTS (?)</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>1.4. Milestone do issue</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: Se o issue faz parte de um conjunto maior de tarefas ou projeto, você pode adicionar o issue a um milestone.</t>
+    </r>
+  </si>
+  <si>
+    <t>Implementation</t>
+  </si>
+  <si>
+    <t>Initial Considerations</t>
+  </si>
+  <si>
+    <t>OBS</t>
   </si>
 </sst>
 </file>
@@ -392,7 +432,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -411,8 +451,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -435,11 +481,48 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -493,6 +576,30 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1165,17 +1272,17 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{662486F5-DD9A-4C28-87E7-50C66D2DE293}">
-  <dimension ref="A1:I45"/>
+  <dimension ref="A1:I46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
   <cols>
     <col min="1" max="1" width="56.04296875" customWidth="1"/>
-    <col min="2" max="2" width="17.86328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.08984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.26953125" customWidth="1"/>
+    <col min="3" max="3" width="16.08984375" customWidth="1"/>
     <col min="4" max="4" width="13.1328125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.453125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10.08984375" bestFit="1" customWidth="1"/>
@@ -1589,150 +1696,257 @@
         <v>69</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.75">
+    <row r="21" spans="1:7" ht="14.75" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A21" s="18" t="s">
         <v>74</v>
       </c>
+      <c r="B21" s="25" t="s">
+        <v>101</v>
+      </c>
+      <c r="C21" s="22" t="s">
+        <v>100</v>
+      </c>
+      <c r="D21" s="25" t="s">
+        <v>102</v>
+      </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A22" s="18"/>
+      <c r="B22" s="26"/>
+      <c r="C22" s="23"/>
+      <c r="D22" s="26"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.75">
-      <c r="A23" s="15" t="s">
+      <c r="A23" s="21" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="24" spans="1:7" ht="44.25" x14ac:dyDescent="0.75">
+      <c r="B23" s="27"/>
+      <c r="C23" s="24"/>
+      <c r="D23" s="27"/>
+    </row>
+    <row r="24" spans="1:7" ht="33.75" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A24" s="15" t="s">
         <v>76</v>
       </c>
-      <c r="B24" t="s">
-        <v>94</v>
+      <c r="B24" s="15" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="29.5" x14ac:dyDescent="0.75">
       <c r="A25" s="15" t="s">
         <v>77</v>
       </c>
-      <c r="B25" t="s">
-        <v>94</v>
+      <c r="B25" s="15" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="44.25" x14ac:dyDescent="0.75">
       <c r="A26" s="15" t="s">
         <v>78</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B26" s="15" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" ht="35" customHeight="1" x14ac:dyDescent="0.75">
+      <c r="A27" s="15" t="s">
+        <v>99</v>
+      </c>
+      <c r="B27" s="15" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" ht="29.5" x14ac:dyDescent="0.75">
+      <c r="A28" s="15" t="s">
+        <v>88</v>
+      </c>
+      <c r="B28" s="15" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" ht="29.5" x14ac:dyDescent="0.75">
+      <c r="A29" s="15" t="s">
+        <v>89</v>
+      </c>
+      <c r="B29" s="15" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" ht="29.5" x14ac:dyDescent="0.75">
+      <c r="A30" s="15" t="s">
+        <v>90</v>
+      </c>
+      <c r="B30" s="15" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.75">
+      <c r="A31" s="21" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="27" spans="1:7" ht="44.25" x14ac:dyDescent="0.75">
-      <c r="A27" s="15" t="s">
-        <v>79</v>
-      </c>
-      <c r="B27" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.75">
-      <c r="A28" s="15" t="s">
-        <v>91</v>
-      </c>
-      <c r="B28" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.75">
-      <c r="A29" s="15" t="s">
-        <v>92</v>
-      </c>
-      <c r="B29" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.75">
-      <c r="A30" s="15" t="s">
-        <v>93</v>
-      </c>
-      <c r="B30" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.75">
-      <c r="A31" s="15" t="s">
-        <v>80</v>
-      </c>
+      <c r="B31" s="15"/>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A32" s="15" t="s">
+        <v>79</v>
+      </c>
+      <c r="B32" s="15"/>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.75">
+      <c r="A33" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="B33" s="15"/>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.75">
+      <c r="A34" s="21" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.75">
-      <c r="A33" s="15" t="s">
+      <c r="B34" s="15"/>
+    </row>
+    <row r="35" spans="1:2" ht="44.25" x14ac:dyDescent="0.75">
+      <c r="A35" s="15" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.75">
-      <c r="A34" s="15" t="s">
+      <c r="B35" s="15"/>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.75">
+      <c r="A36" s="21" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="35" spans="1:1" ht="44.25" x14ac:dyDescent="0.75">
-      <c r="A35" s="15" t="s">
+      <c r="B36" s="15"/>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.75">
+      <c r="A37" s="21" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.75">
-      <c r="A36" s="15" t="s">
+      <c r="B37" s="15"/>
+    </row>
+    <row r="38" spans="1:2" ht="29.5" x14ac:dyDescent="0.75">
+      <c r="A38" s="15" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.75">
-      <c r="A37" s="15" t="s">
+      <c r="B38" s="15"/>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.75">
+      <c r="A39" s="15" t="s">
+        <v>97</v>
+      </c>
+      <c r="B39" s="15"/>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.75">
+      <c r="A40" s="21" t="s">
+        <v>98</v>
+      </c>
+      <c r="B40" s="15"/>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.75">
+      <c r="A41" s="21" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="38" spans="1:1" ht="29.5" x14ac:dyDescent="0.75">
-      <c r="A38" s="15" t="s">
+      <c r="B41" s="15"/>
+    </row>
+    <row r="42" spans="1:2" ht="44.25" x14ac:dyDescent="0.75">
+      <c r="A42" s="15" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.75">
-      <c r="A39" s="15" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.75">
-      <c r="A40" s="15" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="41" spans="1:1" ht="44.25" x14ac:dyDescent="0.75">
-      <c r="A41" s="15" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="42" spans="1:1" ht="18.5" x14ac:dyDescent="0.75">
-      <c r="A42" s="17"/>
-    </row>
-    <row r="43" spans="1:1" ht="18.5" x14ac:dyDescent="0.75">
-      <c r="A43" s="17"/>
-    </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.75">
-      <c r="A44" s="15"/>
-    </row>
-    <row r="45" spans="1:1" ht="18.5" x14ac:dyDescent="0.75">
-      <c r="A45" s="16"/>
+      <c r="B42" s="15"/>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.75">
+      <c r="A43" s="20" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" ht="18.5" x14ac:dyDescent="0.75">
+      <c r="A44" s="17"/>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.75">
+      <c r="A45" s="15"/>
+    </row>
+    <row r="46" spans="1:2" ht="18.5" x14ac:dyDescent="0.75">
+      <c r="A46" s="16"/>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="8">
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="A9:A10"/>
     <mergeCell ref="B9:G9"/>
     <mergeCell ref="B1:I1"/>
     <mergeCell ref="A21:A22"/>
+    <mergeCell ref="B21:B23"/>
+    <mergeCell ref="C21:C23"/>
+    <mergeCell ref="D21:D23"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC8091F9-8276-4EBA-959C-9675E2CE363F}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K6" sqref="K6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <sheetData/>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3EE9E530-6434-40D5-85A1-15A72B92A7C4}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H5" sqref="H5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <sheetData/>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49357937-32BA-4486-B49A-4437D20089DD}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I6" sqref="I6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <sheetData/>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BBD53C8E-C643-4BCE-BF25-2F68FDF70BBB}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <sheetData/>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA838CB1-E8D0-4DF8-AF2E-6EB4C9BF74C6}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J6" sqref="J6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <sheetData/>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
 </file>
</xml_diff>